<commit_message>
Add instruction rows and columns feature
- Filter rows starting with # during CSV processing
- Filter columns with names starting with # during JSON conversion
- Update Excel template with # Instructions column and example rows
- Document feature in Google Sheets guide and CHANGELOG
</commit_message>
<xml_diff>
--- a/docs/google_sheets_integration/telar-template.xlsx
+++ b/docs/google_sheets_integration/telar-template.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,13 +31,23 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00666666"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0F0F0"/>
+        <bgColor rgb="00F0F0F0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -58,11 +68,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +459,11 @@
           <t>value</t>
         </is>
       </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t># Instructions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -459,6 +476,11 @@
           <t>Your Exhibition Title</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Short descriptive title (under 60 chars)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -471,148 +493,232 @@
           <t>A brief description of your exhibition</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Row 2 description</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>author</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Your Name or Institution</t>
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t># EXAMPLE</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>This entire row is ignored</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Rows starting with # are skipped during processing</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>author</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>contact@example.com</t>
+          <t>Your Name or Institution</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Individual or organization name</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>primary_color</t>
+          <t>email</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>#2c3e50</t>
+          <t>contact@example.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Row 4 description</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>secondary_color</t>
+          <t>primary_color</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>#8b4513</t>
+          <t>#2c3e50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Row 5 description</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>font_headings</t>
+          <t>secondary_color</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Playfair Display, serif</t>
+          <t>#8b4513</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Row 6 description</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>font_body</t>
+          <t>font_headings</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Source Sans Pro, sans-serif</t>
+          <t>Playfair Display, serif</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Row 7 description</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>font_body</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Source Sans Pro, sans-serif</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Row 8 description</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>logo</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>/assets/images/site/logo.png</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Row 9 description</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>STORIES</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Row 10 description</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Example Telar Story</t>
+          <t>STORIES</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Row 11 description</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Showcase of Telar features</t>
+          <t>Example Telar Story</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Row 12 description</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Chapter 3</t>
+          <t>Showcase of Telar features</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Row 13 description</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Chapter 3</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Row 14 description</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Row 15 description</t>
         </is>
       </c>
     </row>
@@ -627,7 +733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,6 +797,11 @@
           <t>thumbnail</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t># Instructions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -728,7 +839,6 @@
           <t>Copper engraving</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>Huntington Library</t>
@@ -739,7 +849,11 @@
           <t>Huntington Digital Library</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Object 1 - ensure unique object_id</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -757,7 +871,6 @@
           <t>A legal map/painting used as evidence in a land ownership dispute between the crown prosecutor and Francisco Maldonado y Mendoza over land in the Bogotá savannah.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>Juan de Aguilar Rendón (painter) and Alonso Ruiz Gadálmez (guarantor)</t>
@@ -773,7 +886,6 @@
           <t>Oil on canvas, cartographic painting</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>Archivo General de Indias</t>
@@ -784,70 +896,54 @@
           <t>Archivo General de Indias, Seville</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Object 2 - ensure unique object_id</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>example-muisca-goldwork</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Votive Figure in the Shape of a Residential Compound (Cercado)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Gold votive figure from the Muisca culture, demonstrating sophisticated metalworking techniques and ritual practices.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Unknown Muisca Artist</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>600-1600</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Gold alloy</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Museo del Oro</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Museo del Oro, Bogotá. Registration Number: O08319</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t># NOTE</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Add section breaks between object types</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="3" t="n"/>
+      <c r="F4" s="3" t="n"/>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="3" t="n"/>
+      <c r="I4" s="3" t="n"/>
+      <c r="J4" s="3" t="n"/>
+      <c r="K4" s="3" t="n"/>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>Rows starting with # are ignored</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>example-ceramic-figure</t>
+          <t>example-muisca-goldwork</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Anthropomorphic Ceramic Figure</t>
+          <t>Votive Figure in the Shape of a Residential Compound (Cercado)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ceramic figure from the Muisca period representing indigenous material culture and ritual practices before Spanish colonization.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>Gold votive figure from the Muisca culture, demonstrating sophisticated metalworking techniques and ritual practices.</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Unknown Muisca Artist</t>
@@ -855,15 +951,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Pre-colonial era</t>
+          <t>600-1600</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Ceramic</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>Gold alloy</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>Museo del Oro</t>
@@ -871,63 +966,108 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Museo del Oro, Bogotá</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr"/>
+          <t>Museo del Oro, Bogotá. Registration Number: O08319</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Object 3 - ensure unique object_id</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>example-ceramic-figure</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Anthropomorphic Ceramic Figure</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ceramic figure from the Muisca period representing indigenous material culture and ritual practices before Spanish colonization.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Unknown Muisca Artist</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pre-colonial era</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ceramic</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Museo del Oro</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Museo del Oro, Bogotá</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>example-piedrahita-title_page</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Historia general de la conqvistas del nvevo reyno de Granada</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Title page with portrait medallions of seven indigenous rulers or caciques (Sacuan, Sugamuxi, Nemeguene, Vbaqui, Saquesazippa, Thysquesuca, and Guatabita), four battle scenes (battles of Choconta, las Bueltas, Portachuelo, and Voqueron), and two coats of arms.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>https://jcb.lunaimaging.com/luna/servlet/iiif/m/JCB~1~1~278~100020/manifest</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Fernández de Piedrahita, Lucas (1624-1688); Engraved by Joseph Mulder</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>1688</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Engraving, ink on paper</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>28.6 x 19.7 cm</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>John Carter Brown Library</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>John Carter Brown Library, Brown University, Providence, R.I.</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -940,7 +1080,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,6 +1144,11 @@
           <t>layer2_file</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t># Instructions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1033,16 +1178,19 @@
           <t>This 1614 map was created as legal evidence in a land ownership dispute presented by the crown prosecutor against Francisco Maldonado y Mendoza.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>story1/step1-layer1.md</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>story1/step1-layer2.md</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Step 1 notes and reminders</t>
         </is>
       </c>
     </row>
@@ -1074,10 +1222,11 @@
           <t>The map depicts the Bogotá savannah, a high plateau in the northern Andes originally occupied by the Indigenous Muisca people.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Step 2 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1107,55 +1256,86 @@
           <t>This unique 'legal painting' functions as both map and landscape art, rare for being signed by its creator Juan de Aguilar Rendón.</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>story1/step3-layer1.md</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>story1/step3-layer2.md</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Step 3 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t># SECTION</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Use instruction rows to add section breaks</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>This row is skipped - useful for TODOs</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>example-bogota-1614</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>0.6</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>0.7</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>2.2</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Who were the owners of this land?</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>The land belonged to Francisco Maldonado y Mendoza and became the center of the Marquisate of San Jorge.</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>story1/step4-layer1.md</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Step 4 notes and reminders</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1168,7 +1348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1232,6 +1412,11 @@
           <t>layer2_file</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t># Instructions</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1261,14 +1446,16 @@
           <t>Telar works with IIIF images from any institution. This map comes from the Huntington Library's digital collection.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>story2/step1-layer1.md</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Step 1 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1298,14 +1485,16 @@
           <t>Yes! Telar can auto-generate IIIF tiles from your own images, giving you the same zoom and pan capabilities as materials hosted externally.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>story2/step2-layer1.md</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Step 2 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1345,65 +1534,45 @@
           <t>story2/step3-layer1.md</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Step 3 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>example-bogota-1614</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Can I add layers of information?</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Yes! Telar uses a two-panel system for progressive disclosure. Layer 1 provides context, Layer 2 offers deeper analysis.</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Context</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>story2/step4-layer1.md</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Deep Dive</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>story2/step4-layer2.md</t>
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t># SECTION</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Use instruction rows to add section breaks</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>This row is skipped - useful for TODOs</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>example-piedrahita-title_page</t>
+          <t>example-bogota-1614</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1413,30 +1582,47 @@
         <v>0.5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>What can I do with pan and zoom?</t>
+          <t>Can I add layers of information?</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Telar gives you precise control over your reader's view. Let's explore this ornate title page from the John Carter Brown Library.</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Yes! Telar uses a two-panel system for progressive disclosure. Layer 1 provides context, Layer 2 offers deeper analysis.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Context</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>story2/step5-layer1.md</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+          <t>story2/step4-layer1.md</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Deep Dive</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>story2/step4-layer2.md</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Step 4 notes and reminders</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1444,32 +1630,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Can I zoom to specific details?</t>
+          <t>What can I do with pan and zoom?</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Yes! Each step defines x, y coordinates and zoom level. Here we've zoomed to one of the portrait medallions of an indigenous ruler.</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+          <t>Telar gives you precise control over your reader's view. Let's explore this ornate title page from the John Carter Brown Library.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>story2/step5-layer1.md</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1477,32 +1664,28 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.49</v>
+        <v>0.25</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="E8" t="n">
         <v>4</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Can I pan across the same image?</t>
+          <t>Can I zoom to specific details?</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Absolutely - notice how we've panned to a different medallion while staying at the same zoom level. This guides your reader's attention across the image.</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+          <t>Yes! Each step defines x, y coordinates and zoom level. Here we've zoomed to one of the portrait medallions of an indigenous ruler.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1510,32 +1693,28 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.75</v>
+        <v>0.49</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>What about zooming to different areas?</t>
+          <t>Can I pan across the same image?</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>You can combine panning and zooming freely. Here's one of the battle scenes depicted in the border decorations.</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+          <t>Absolutely - notice how we've panned to a different medallion while staying at the same zoom level. This guides your reader's attention across the image.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1543,36 +1722,32 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Do all steps need additional panels?</t>
+          <t>What about zooming to different areas?</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>No! Some steps work perfectly with just the question and answer, while others benefit from detailed explanations in the side panels.</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+          <t>You can combine panning and zooming freely. Here's one of the battle scenes depicted in the border decorations.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>example-terrafirma-map</t>
+          <t>example-piedrahita-title_page</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1586,26 +1761,53 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Do all steps need additional panels?</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No! Some steps work perfectly with just the question and answer, while others benefit from detailed explanations in the side panels.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>example-terrafirma-map</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>What sorts of stories can I write?</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>You can tell any visual narrative by combining objects, controlling views, formatting text, and embedding rich media like images and videos in panels.</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Storytelling Possibilities</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>story2/step10-layer1.md</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>